<commit_message>
Improved quantity estimation from azure
</commit_message>
<xml_diff>
--- a/grocery_mapping.xlsx
+++ b/grocery_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f45f2a6c0e1abdcf/Dokumente/Count_prototype/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\OneDrive\Dokumente\Count_prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="560" documentId="13_ncr:1_{CE627C6A-5BB3-41B3-AC5A-E60A0477CE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CEABBCE-196E-4AF8-B30C-BB9E09F890A5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE91FE44-BF38-44FB-844C-1B53654C778A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{9CEB87A9-AAE3-4144-8460-A009C5F567C6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Carbon_footprint" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Carbon_footprint!$A$1:$F$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Carbon_footprint!$A$1:$F$197</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="227">
   <si>
     <t>Hähnchen Fleisch</t>
   </si>
@@ -682,6 +682,42 @@
   </si>
   <si>
     <t>Soy flour</t>
+  </si>
+  <si>
+    <t>Rosenkohl</t>
+  </si>
+  <si>
+    <t>Garnelen</t>
+  </si>
+  <si>
+    <t>Bordeaux</t>
+  </si>
+  <si>
+    <t>Kokosöl</t>
+  </si>
+  <si>
+    <t>Dt. Markenbut</t>
+  </si>
+  <si>
+    <t>Nuss-Nougat Creme</t>
+  </si>
+  <si>
+    <t>Palmöl</t>
+  </si>
+  <si>
+    <t>Rioja</t>
+  </si>
+  <si>
+    <t>Ahornsirup</t>
+  </si>
+  <si>
+    <t>Kohlrabi</t>
+  </si>
+  <si>
+    <t>Capellini</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Muesli</t>
   </si>
 </sst>
 </file>
@@ -1047,23 +1083,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D95502D-50C3-4DDD-A8F3-7C8C0FCBD78D}">
-  <dimension ref="A1:F189"/>
+  <dimension ref="A1:F198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="F188" sqref="F188"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -1083,7 +1119,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1101,7 +1137,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1155,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1173,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1155,7 +1191,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1209,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1227,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1209,7 +1245,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1227,7 +1263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1245,7 +1281,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1299,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1281,7 +1317,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1299,7 +1335,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1317,7 +1353,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1335,7 +1371,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1353,7 +1389,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1371,7 +1407,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1389,7 +1425,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1407,7 +1443,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1425,7 +1461,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1443,7 +1479,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1461,7 +1497,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1479,7 +1515,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1497,7 +1533,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1515,7 +1551,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1533,7 +1569,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1551,7 +1587,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1569,7 +1605,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1587,7 +1623,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1605,7 +1641,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1623,7 +1659,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1641,7 +1677,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1659,7 +1695,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1677,7 +1713,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1698,7 +1734,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1716,7 +1752,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1734,7 +1770,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1752,7 +1788,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1770,7 +1806,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1791,7 +1827,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1809,7 +1845,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1827,7 +1863,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1845,7 +1881,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -1863,7 +1899,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1881,7 +1917,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -1902,7 +1938,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +1956,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -1938,7 +1974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -1959,7 +1995,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1977,7 +2013,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1998,7 +2034,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2019,7 +2055,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -2037,7 +2073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2058,7 +2094,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2076,7 +2112,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -2097,7 +2133,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2115,7 +2151,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2133,7 +2169,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2151,7 +2187,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2172,7 +2208,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2193,7 +2229,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2214,7 +2250,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2232,7 +2268,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>173</v>
       </c>
@@ -2253,7 +2289,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2274,7 +2310,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2292,7 +2328,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2310,7 +2346,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2328,7 +2364,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2346,7 +2382,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2364,7 +2400,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2382,7 +2418,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2400,7 +2436,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2418,7 +2454,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2439,7 +2475,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2457,7 +2493,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2475,7 +2511,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2496,7 +2532,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2517,7 +2553,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>188</v>
       </c>
@@ -2538,7 +2574,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -2559,7 +2595,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -2580,7 +2616,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -2601,7 +2637,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -2619,7 +2655,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -2640,7 +2676,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -2661,7 +2697,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -2682,7 +2718,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -2703,7 +2739,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -2724,7 +2760,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -2745,7 +2781,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -2766,7 +2802,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -2787,7 +2823,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -2808,7 +2844,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>103</v>
       </c>
@@ -2829,7 +2865,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -2847,7 +2883,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -2868,7 +2904,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -2886,7 +2922,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -2904,7 +2940,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -2925,7 +2961,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -2946,7 +2982,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -2967,7 +3003,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -2985,7 +3021,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>172</v>
       </c>
@@ -3003,7 +3039,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>118</v>
       </c>
@@ -3024,7 +3060,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -3045,7 +3081,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -3066,7 +3102,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -3087,7 +3123,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -3108,7 +3144,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -3126,7 +3162,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -3147,7 +3183,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -3168,7 +3204,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -3189,7 +3225,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -3210,7 +3246,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -3228,7 +3264,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -3249,7 +3285,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -3267,7 +3303,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -3285,7 +3321,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -3306,7 +3342,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>137</v>
       </c>
@@ -3327,7 +3363,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -3348,7 +3384,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>138</v>
       </c>
@@ -3369,7 +3405,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>139</v>
       </c>
@@ -3390,7 +3426,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>140</v>
       </c>
@@ -3408,7 +3444,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>141</v>
       </c>
@@ -3429,7 +3465,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>142</v>
       </c>
@@ -3450,7 +3486,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>143</v>
       </c>
@@ -3468,7 +3504,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>144</v>
       </c>
@@ -3489,7 +3525,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>170</v>
       </c>
@@ -3510,7 +3546,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>145</v>
       </c>
@@ -3531,7 +3567,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>146</v>
       </c>
@@ -3552,7 +3588,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>147</v>
       </c>
@@ -3573,7 +3609,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>148</v>
       </c>
@@ -3591,7 +3627,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -3612,7 +3648,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>150</v>
       </c>
@@ -3633,7 +3669,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>152</v>
       </c>
@@ -3654,7 +3690,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>153</v>
       </c>
@@ -3675,7 +3711,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>154</v>
       </c>
@@ -3696,7 +3732,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>155</v>
       </c>
@@ -3717,7 +3753,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>156</v>
       </c>
@@ -3735,7 +3771,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>157</v>
       </c>
@@ -3753,7 +3789,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>158</v>
       </c>
@@ -3771,7 +3807,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>159</v>
       </c>
@@ -3789,7 +3825,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>160</v>
       </c>
@@ -3810,7 +3846,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>161</v>
       </c>
@@ -3828,7 +3864,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>162</v>
       </c>
@@ -3849,7 +3885,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>163</v>
       </c>
@@ -3867,7 +3903,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>164</v>
       </c>
@@ -3888,7 +3924,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>166</v>
       </c>
@@ -3906,7 +3942,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>167</v>
       </c>
@@ -3927,7 +3963,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>168</v>
       </c>
@@ -3948,7 +3984,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>171</v>
       </c>
@@ -3969,7 +4005,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>174</v>
       </c>
@@ -3987,7 +4023,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>175</v>
       </c>
@@ -4005,7 +4041,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>176</v>
       </c>
@@ -4026,7 +4062,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>177</v>
       </c>
@@ -4044,7 +4080,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>178</v>
       </c>
@@ -4062,7 +4098,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>179</v>
       </c>
@@ -4080,7 +4116,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>180</v>
       </c>
@@ -4098,7 +4134,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>181</v>
       </c>
@@ -4116,7 +4152,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>182</v>
       </c>
@@ -4138,7 +4174,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>183</v>
       </c>
@@ -4149,14 +4185,14 @@
         <v>700</v>
       </c>
       <c r="D160">
-        <f t="shared" ref="D160:D187" si="2">B160*(C160/100)</f>
+        <f t="shared" ref="D160:D198" si="2">B160*(C160/100)</f>
         <v>735</v>
       </c>
       <c r="F160" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>184</v>
       </c>
@@ -4174,7 +4210,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>185</v>
       </c>
@@ -4192,7 +4228,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>186</v>
       </c>
@@ -4210,7 +4246,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>187</v>
       </c>
@@ -4231,7 +4267,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>189</v>
       </c>
@@ -4249,7 +4285,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>190</v>
       </c>
@@ -4273,7 +4309,7 @@
         <v>Milchprodukte / Eier</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>191</v>
       </c>
@@ -4297,7 +4333,7 @@
         <v>Fleisch / Fisch</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>192</v>
       </c>
@@ -4321,7 +4357,7 @@
         <v>Fleisch / Fisch</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>193</v>
       </c>
@@ -4345,7 +4381,7 @@
         <v>Sonstiges</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>194</v>
       </c>
@@ -4369,7 +4405,7 @@
         <v>Fleisch / Fisch</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>197</v>
       </c>
@@ -4393,7 +4429,7 @@
         <v>Sonstiges</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>198</v>
       </c>
@@ -4417,7 +4453,7 @@
         <v>Milchprodukte / Eier</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>199</v>
       </c>
@@ -4435,12 +4471,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>196</v>
       </c>
       <c r="B174" s="2">
-        <f>VLOOKUP(E174,A:B,2,FALSE)</f>
+        <f t="shared" ref="B174:B181" si="6">VLOOKUP(E174,A:B,2,FALSE)</f>
         <v>23</v>
       </c>
       <c r="C174">
@@ -4459,12 +4495,12 @@
         <v>Obst / Gemüse</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>201</v>
       </c>
       <c r="B175" s="2">
-        <f>VLOOKUP(E175,A:B,2,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>6.14</v>
       </c>
       <c r="C175">
@@ -4482,12 +4518,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>209</v>
       </c>
       <c r="B176" s="2">
-        <f>VLOOKUP(E176,A:B,2,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>235</v>
       </c>
       <c r="C176">
@@ -4504,228 +4540,446 @@
         <v>80</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="B177" s="2">
-        <f>VLOOKUP(E177,A:B,2,FALSE)</f>
-        <v>178</v>
+        <f t="shared" si="6"/>
+        <v>303</v>
       </c>
       <c r="C177">
-        <v>200</v>
+        <f>VLOOKUP(E177,A:C,3,FALSE)</f>
+        <v>250</v>
       </c>
       <c r="D177">
         <f t="shared" si="2"/>
-        <v>356</v>
+        <v>757.5</v>
       </c>
       <c r="E177" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="F177" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>195</v>
-      </c>
-      <c r="B178" s="1">
-        <v>150</v>
+        <v>217</v>
+      </c>
+      <c r="B178" s="2">
+        <f t="shared" si="6"/>
+        <v>37</v>
       </c>
       <c r="C178">
-        <v>69</v>
+        <f>VLOOKUP(E178,A:C,3,FALSE)</f>
+        <v>750</v>
       </c>
       <c r="D178">
         <f t="shared" si="2"/>
-        <v>103.49999999999999</v>
+        <v>277.5</v>
+      </c>
+      <c r="E178" t="s">
+        <v>19</v>
       </c>
       <c r="F178" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>200</v>
-      </c>
-      <c r="B179" s="1">
-        <v>168</v>
+        <v>222</v>
+      </c>
+      <c r="B179" s="2">
+        <f t="shared" si="6"/>
+        <v>37</v>
       </c>
       <c r="C179">
-        <v>120</v>
+        <f>VLOOKUP(E179,A:C,3,FALSE)</f>
+        <v>750</v>
       </c>
       <c r="D179">
         <f t="shared" si="2"/>
-        <v>201.6</v>
+        <v>277.5</v>
+      </c>
+      <c r="E179" t="s">
+        <v>19</v>
       </c>
       <c r="F179" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="B180" s="2">
-        <v>22</v>
+        <f t="shared" si="6"/>
+        <v>32</v>
       </c>
       <c r="C180">
-        <v>200</v>
+        <f>VLOOKUP(E180,A:C,3,FALSE)</f>
+        <v>500</v>
       </c>
       <c r="D180">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>160</v>
+      </c>
+      <c r="E180" t="s">
+        <v>11</v>
       </c>
       <c r="F180" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>203</v>
-      </c>
-      <c r="B181" s="1">
-        <v>41</v>
+        <v>208</v>
+      </c>
+      <c r="B181" s="2">
+        <f t="shared" si="6"/>
+        <v>178</v>
       </c>
       <c r="C181">
         <v>200</v>
       </c>
       <c r="D181">
         <f t="shared" si="2"/>
-        <v>82</v>
+        <v>356</v>
+      </c>
+      <c r="E181" t="s">
+        <v>74</v>
       </c>
       <c r="F181" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B182" s="1">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="C182">
-        <v>250</v>
+        <v>69</v>
       </c>
       <c r="D182">
         <f t="shared" si="2"/>
-        <v>62.5</v>
-      </c>
-      <c r="E182" t="s">
-        <v>206</v>
+        <v>103.49999999999999</v>
       </c>
       <c r="F182" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B183" s="1">
-        <v>27</v>
+        <v>168</v>
       </c>
       <c r="C183">
-        <v>250</v>
+        <v>120</v>
       </c>
       <c r="D183">
         <f t="shared" si="2"/>
-        <v>67.5</v>
-      </c>
-      <c r="E183" t="s">
-        <v>207</v>
+        <v>201.6</v>
       </c>
       <c r="F183" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>210</v>
-      </c>
-      <c r="B184" s="1">
-        <v>5.3</v>
+        <v>202</v>
+      </c>
+      <c r="B184" s="2">
+        <v>22</v>
       </c>
       <c r="C184">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D184">
         <f t="shared" si="2"/>
-        <v>13.25</v>
+        <v>44</v>
       </c>
       <c r="F184" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B185" s="1">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="C185">
         <v>200</v>
       </c>
       <c r="D185">
         <f t="shared" si="2"/>
-        <v>172</v>
+        <v>82</v>
       </c>
       <c r="F185" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B186" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C186">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D186">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>62.5</v>
       </c>
       <c r="E186" t="s">
-        <v>54</v>
+        <v>206</v>
       </c>
       <c r="F186" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B187" s="1">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C187">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="D187">
         <f t="shared" si="2"/>
-        <v>365</v>
+        <v>67.5</v>
       </c>
       <c r="E187" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F187" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B188" s="1"/>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B189" s="1"/>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>210</v>
+      </c>
+      <c r="B188" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="C188">
+        <v>250</v>
+      </c>
+      <c r="D188">
+        <f t="shared" si="2"/>
+        <v>13.25</v>
+      </c>
+      <c r="F188" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>211</v>
+      </c>
+      <c r="B189" s="1">
+        <v>86</v>
+      </c>
+      <c r="C189">
+        <v>200</v>
+      </c>
+      <c r="D189">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+      <c r="F189" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>212</v>
+      </c>
+      <c r="B190" s="1">
+        <v>15</v>
+      </c>
+      <c r="C190">
+        <v>200</v>
+      </c>
+      <c r="D190">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E190" t="s">
+        <v>54</v>
+      </c>
+      <c r="F190" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>213</v>
+      </c>
+      <c r="B191" s="1">
+        <v>73</v>
+      </c>
+      <c r="C191">
+        <v>500</v>
+      </c>
+      <c r="D191">
+        <f t="shared" si="2"/>
+        <v>365</v>
+      </c>
+      <c r="E191" t="s">
+        <v>214</v>
+      </c>
+      <c r="F191" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>215</v>
+      </c>
+      <c r="B192" s="1">
+        <v>14</v>
+      </c>
+      <c r="C192">
+        <v>750</v>
+      </c>
+      <c r="D192">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="F192" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>216</v>
+      </c>
+      <c r="B193" s="1">
+        <v>256</v>
+      </c>
+      <c r="C193">
+        <v>250</v>
+      </c>
+      <c r="D193">
+        <f t="shared" si="2"/>
+        <v>640</v>
+      </c>
+      <c r="F193" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>218</v>
+      </c>
+      <c r="B194" s="1">
+        <v>79</v>
+      </c>
+      <c r="C194">
+        <v>250</v>
+      </c>
+      <c r="D194">
+        <f t="shared" si="2"/>
+        <v>197.5</v>
+      </c>
+      <c r="F194" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>220</v>
+      </c>
+      <c r="B195" s="1">
+        <v>119</v>
+      </c>
+      <c r="C195">
+        <v>500</v>
+      </c>
+      <c r="D195">
+        <f t="shared" si="2"/>
+        <v>595</v>
+      </c>
+      <c r="E195" t="s">
+        <v>221</v>
+      </c>
+      <c r="F195" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>223</v>
+      </c>
+      <c r="B196" s="1">
+        <v>37</v>
+      </c>
+      <c r="C196">
+        <v>250</v>
+      </c>
+      <c r="D196">
+        <f t="shared" si="2"/>
+        <v>92.5</v>
+      </c>
+      <c r="F196" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>224</v>
+      </c>
+      <c r="B197" s="1">
+        <v>6.93</v>
+      </c>
+      <c r="C197">
+        <v>500</v>
+      </c>
+      <c r="D197">
+        <f t="shared" si="2"/>
+        <v>34.65</v>
+      </c>
+      <c r="F197" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>226</v>
+      </c>
+      <c r="B198" s="1">
+        <v>21</v>
+      </c>
+      <c r="C198">
+        <v>700</v>
+      </c>
+      <c r="D198">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="E198" t="s">
+        <v>136</v>
+      </c>
+      <c r="F198" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F178" xr:uid="{9D95502D-50C3-4DDD-A8F3-7C8C0FCBD78D}"/>
+  <autoFilter ref="A1:F197" xr:uid="{9D95502D-50C3-4DDD-A8F3-7C8C0FCBD78D}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
FIx wrong mapping behavior for search
</commit_message>
<xml_diff>
--- a/grocery_mapping.xlsx
+++ b/grocery_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f45f2a6c0e1abdcf/Dokumente/Count_prototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="749" documentId="8_{9643AA81-64B7-47EB-92E8-933800F6D933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{949C3F5E-45C5-4DA6-BDC7-C79F7319EDB3}"/>
+  <xr:revisionPtr revIDLastSave="753" documentId="8_{9643AA81-64B7-47EB-92E8-933800F6D933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F59F17E7-CCCA-4CD6-83F3-27091F030B84}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1575D379-9279-429E-8A00-2E1BF894E283}"/>
+    <workbookView xWindow="9450" yWindow="1905" windowWidth="28800" windowHeight="11265" xr2:uid="{1575D379-9279-429E-8A00-2E1BF894E283}"/>
   </bookViews>
   <sheets>
     <sheet name="Grocery_footprint" sheetId="2" r:id="rId1"/>
@@ -3652,8 +3652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D520EB4-329C-42ED-AA24-ED945CB71FA9}">
   <dimension ref="A1:F1056"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
-      <selection activeCell="A454" sqref="A454:A457"/>
+    <sheetView tabSelected="1" topLeftCell="A773" workbookViewId="0">
+      <selection activeCell="A778" sqref="A778:F778"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding pfand und leergut
</commit_message>
<xml_diff>
--- a/grocery_mapping.xlsx
+++ b/grocery_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f45f2a6c0e1abdcf/Dokumente/Count_prototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="783" documentId="8_{9643AA81-64B7-47EB-92E8-933800F6D933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D0D6207-8B05-44D9-8226-54D47F1CD0B6}"/>
+  <xr:revisionPtr revIDLastSave="800" documentId="8_{9643AA81-64B7-47EB-92E8-933800F6D933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3677D1F-D11A-4580-B192-6D266AD7B0AE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1575D379-9279-429E-8A00-2E1BF894E283}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2687" uniqueCount="1080">
   <si>
     <t>typical_weight</t>
   </si>
@@ -3266,6 +3266,18 @@
   </si>
   <si>
     <t>Steak</t>
+  </si>
+  <si>
+    <t>Leergut</t>
+  </si>
+  <si>
+    <t>Leerg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEERG. MW </t>
+  </si>
+  <si>
+    <t>Pfand</t>
   </si>
 </sst>
 </file>
@@ -3675,10 +3687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D520EB4-329C-42ED-AA24-ED945CB71FA9}">
-  <dimension ref="A1:F1056"/>
+  <dimension ref="A1:F1060"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
-      <selection activeCell="E460" sqref="E460"/>
+    <sheetView tabSelected="1" topLeftCell="A1045" workbookViewId="0">
+      <selection activeCell="F1061" sqref="F1061"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23330,6 +23342,80 @@
         <v>98</v>
       </c>
       <c r="F1056" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1057" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1057" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1057" s="6">
+        <v>0</v>
+      </c>
+      <c r="D1057" s="3">
+        <v>0</v>
+      </c>
+      <c r="F1057" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1058" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B1058" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1058" s="6">
+        <v>0</v>
+      </c>
+      <c r="D1058" s="3">
+        <v>0</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F1058" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1059" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1059" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1059" s="6">
+        <v>0</v>
+      </c>
+      <c r="D1059" s="3">
+        <v>0</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F1059" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1060" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1060" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1060" s="6">
+        <v>0</v>
+      </c>
+      <c r="D1060" s="3">
+        <v>0</v>
+      </c>
+      <c r="F1060" t="s">
         <v>382</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing uneven quantity bug
</commit_message>
<xml_diff>
--- a/grocery_mapping.xlsx
+++ b/grocery_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f45f2a6c0e1abdcf/Dokumente/Count_prototype/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\OneDrive\Dokumente\Count_prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="800" documentId="8_{9643AA81-64B7-47EB-92E8-933800F6D933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3677D1F-D11A-4580-B192-6D266AD7B0AE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9607D0-673F-4D0A-A4B0-EFEF541DDBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1575D379-9279-429E-8A00-2E1BF894E283}"/>
   </bookViews>
@@ -3689,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D520EB4-329C-42ED-AA24-ED945CB71FA9}">
   <dimension ref="A1:F1060"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1045" workbookViewId="0">
-      <selection activeCell="F1061" sqref="F1061"/>
+    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
+      <selection activeCell="D487" sqref="D487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12045,7 +12045,7 @@
         <v>400</v>
       </c>
       <c r="D486" s="3">
-        <v>15883.86</v>
+        <v>1588</v>
       </c>
       <c r="F486" t="s">
         <v>382</v>

</xml_diff>